<commit_message>
Task 3 Forecasting Complete (via Azure Function APIs)
</commit_message>
<xml_diff>
--- a/RESULTS/task2Submission/all_scores_final.xlsx
+++ b/RESULTS/task2Submission/all_scores_final.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbowc\Documents\GitHub\EnergyCatapultPresumedOpenDataChallange-\RESULTS\task2Submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AF436A-394A-4B7E-A591-F5BFDD282B9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A0B6A-18DC-49DA-8208-C2DFB7F59534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5412" yWindow="2532" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily scores_task1" sheetId="1" r:id="rId1"/>
     <sheet name="Daily scores_task2" sheetId="2" r:id="rId2"/>
     <sheet name="Average_scores" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Average_scores!$C$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Average_scores!$C$2:$C$48</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Average_scores!$C$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Average_scores!$C$2:$C$48</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2134,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:J41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3551,8 +3557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4383,6 +4389,30 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E49">
     <sortCondition descending="1" ref="E1:E49"/>
   </sortState>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>